<commit_message>
Update BDD avec Long. Lat.
</commit_message>
<xml_diff>
--- a/BDD/BDD_Chantier.xlsx
+++ b/BDD/BDD_Chantier.xlsx
@@ -1,44 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moi\Documents\GitHub\WDPII\BDD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlan\Documents\GitHub\WDPII\BDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0B0B38-9AE6-40C6-9B0C-1988A87FDDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140"/>
+    <workbookView xWindow="5660" yWindow="340" windowWidth="13330" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -93,11 +80,17 @@
   <si>
     <t>Décharge sauvage</t>
   </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -160,660 +153,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Quartier mal fréquenté"/>
-      <sheetName val="Quartier aisé"/>
-      <sheetName val="Chantier"/>
-      <sheetName val="Déménagement"/>
-      <sheetName val="Espace verts"/>
-      <sheetName val="Discothèque"/>
-      <sheetName val="Festival"/>
-      <sheetName val="Groupe scolaire"/>
-      <sheetName val="Groupe scolaire + espace vert"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="A2">
-            <v>44927</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Date</v>
-          </cell>
-          <cell r="B1" t="str">
-            <v>Volume</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>Nocivité</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2">
-            <v>44927</v>
-          </cell>
-          <cell r="B2">
-            <v>0</v>
-          </cell>
-          <cell r="C2">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>44934</v>
-          </cell>
-          <cell r="B3">
-            <v>3</v>
-          </cell>
-          <cell r="C3">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>44941</v>
-          </cell>
-          <cell r="B4">
-            <v>3</v>
-          </cell>
-          <cell r="C4">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>44948</v>
-          </cell>
-          <cell r="B5">
-            <v>2</v>
-          </cell>
-          <cell r="C5">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>44955</v>
-          </cell>
-          <cell r="B6">
-            <v>3</v>
-          </cell>
-          <cell r="C6">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>44962</v>
-          </cell>
-          <cell r="B7">
-            <v>3</v>
-          </cell>
-          <cell r="C7">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>44969</v>
-          </cell>
-          <cell r="B8">
-            <v>2</v>
-          </cell>
-          <cell r="C8">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>44976</v>
-          </cell>
-          <cell r="B9">
-            <v>3</v>
-          </cell>
-          <cell r="C9">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>44983</v>
-          </cell>
-          <cell r="B10">
-            <v>3</v>
-          </cell>
-          <cell r="C10">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>44990</v>
-          </cell>
-          <cell r="B11">
-            <v>3</v>
-          </cell>
-          <cell r="C11">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>44997</v>
-          </cell>
-          <cell r="B12">
-            <v>3</v>
-          </cell>
-          <cell r="C12">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>45004</v>
-          </cell>
-          <cell r="B13">
-            <v>3</v>
-          </cell>
-          <cell r="C13">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>45011</v>
-          </cell>
-          <cell r="B14">
-            <v>3</v>
-          </cell>
-          <cell r="C14">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>45018</v>
-          </cell>
-          <cell r="B15">
-            <v>1</v>
-          </cell>
-          <cell r="C15">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>45025</v>
-          </cell>
-          <cell r="B16">
-            <v>2</v>
-          </cell>
-          <cell r="C16">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>45032</v>
-          </cell>
-          <cell r="B17">
-            <v>3</v>
-          </cell>
-          <cell r="C17">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>45039</v>
-          </cell>
-          <cell r="B18">
-            <v>3</v>
-          </cell>
-          <cell r="C18">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>45046</v>
-          </cell>
-          <cell r="B19">
-            <v>3</v>
-          </cell>
-          <cell r="C19">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>45053</v>
-          </cell>
-          <cell r="B20">
-            <v>3</v>
-          </cell>
-          <cell r="C20">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>45060</v>
-          </cell>
-          <cell r="B21">
-            <v>3</v>
-          </cell>
-          <cell r="C21">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>45067</v>
-          </cell>
-          <cell r="B22">
-            <v>2</v>
-          </cell>
-          <cell r="C22">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23">
-            <v>45074</v>
-          </cell>
-          <cell r="B23">
-            <v>2</v>
-          </cell>
-          <cell r="C23">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24">
-            <v>45081</v>
-          </cell>
-          <cell r="B24">
-            <v>1</v>
-          </cell>
-          <cell r="C24">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25">
-            <v>45088</v>
-          </cell>
-          <cell r="B25">
-            <v>2</v>
-          </cell>
-          <cell r="C25">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26">
-            <v>45095</v>
-          </cell>
-          <cell r="B26">
-            <v>2</v>
-          </cell>
-          <cell r="C26">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27">
-            <v>45102</v>
-          </cell>
-          <cell r="B27">
-            <v>2</v>
-          </cell>
-          <cell r="C27">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28">
-            <v>45109</v>
-          </cell>
-          <cell r="B28">
-            <v>1</v>
-          </cell>
-          <cell r="C28">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29">
-            <v>45116</v>
-          </cell>
-          <cell r="B29">
-            <v>1</v>
-          </cell>
-          <cell r="C29">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30">
-            <v>45123</v>
-          </cell>
-          <cell r="B30">
-            <v>1</v>
-          </cell>
-          <cell r="C30">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31">
-            <v>45130</v>
-          </cell>
-          <cell r="B31">
-            <v>1</v>
-          </cell>
-          <cell r="C31">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32">
-            <v>45137</v>
-          </cell>
-          <cell r="B32">
-            <v>0</v>
-          </cell>
-          <cell r="C32">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33">
-            <v>45144</v>
-          </cell>
-          <cell r="B33">
-            <v>1</v>
-          </cell>
-          <cell r="C33">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34">
-            <v>45151</v>
-          </cell>
-          <cell r="B34">
-            <v>2</v>
-          </cell>
-          <cell r="C34">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35">
-            <v>45158</v>
-          </cell>
-          <cell r="B35">
-            <v>2</v>
-          </cell>
-          <cell r="C35">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36">
-            <v>45165</v>
-          </cell>
-          <cell r="B36">
-            <v>1</v>
-          </cell>
-          <cell r="C36">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37">
-            <v>45172</v>
-          </cell>
-          <cell r="B37">
-            <v>0</v>
-          </cell>
-          <cell r="C37">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38">
-            <v>45179</v>
-          </cell>
-          <cell r="B38">
-            <v>1</v>
-          </cell>
-          <cell r="C38">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39">
-            <v>45186</v>
-          </cell>
-          <cell r="B39">
-            <v>0</v>
-          </cell>
-          <cell r="C39">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40">
-            <v>45193</v>
-          </cell>
-          <cell r="B40">
-            <v>0</v>
-          </cell>
-          <cell r="C40">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41">
-            <v>45200</v>
-          </cell>
-          <cell r="B41">
-            <v>0</v>
-          </cell>
-          <cell r="C41">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42">
-            <v>45207</v>
-          </cell>
-          <cell r="B42">
-            <v>0</v>
-          </cell>
-          <cell r="C42">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="A43">
-            <v>45214</v>
-          </cell>
-          <cell r="B43">
-            <v>1</v>
-          </cell>
-          <cell r="C43">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="A44">
-            <v>45221</v>
-          </cell>
-          <cell r="B44">
-            <v>1</v>
-          </cell>
-          <cell r="C44">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="A45">
-            <v>45228</v>
-          </cell>
-          <cell r="B45">
-            <v>1</v>
-          </cell>
-          <cell r="C45">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="A46">
-            <v>45235</v>
-          </cell>
-          <cell r="B46">
-            <v>1</v>
-          </cell>
-          <cell r="C46">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="A47">
-            <v>45242</v>
-          </cell>
-          <cell r="B47">
-            <v>1</v>
-          </cell>
-          <cell r="C47">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="A48">
-            <v>45249</v>
-          </cell>
-          <cell r="B48">
-            <v>2</v>
-          </cell>
-          <cell r="C48">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="A49">
-            <v>45256</v>
-          </cell>
-          <cell r="B49">
-            <v>1</v>
-          </cell>
-          <cell r="C49">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="A50">
-            <v>45263</v>
-          </cell>
-          <cell r="B50">
-            <v>1</v>
-          </cell>
-          <cell r="C50">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="A51">
-            <v>45270</v>
-          </cell>
-          <cell r="B51">
-            <v>1</v>
-          </cell>
-          <cell r="C51">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="A52">
-            <v>45277</v>
-          </cell>
-          <cell r="B52">
-            <v>1</v>
-          </cell>
-          <cell r="C52">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="A53">
-            <v>45284</v>
-          </cell>
-          <cell r="B53">
-            <v>1</v>
-          </cell>
-          <cell r="C53">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="A54">
-            <v>45291</v>
-          </cell>
-          <cell r="B54">
-            <v>2</v>
-          </cell>
-          <cell r="C54">
-            <v>2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Volume</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Volume</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Volume</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Volume</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="8"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1112,16 +451,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1137,14 +476,18 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>44927</v>
       </c>
@@ -1160,14 +503,18 @@
       <c r="E2" s="1">
         <v>579.4</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="F2" s="1">
+        <v>45.64</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.17</v>
+      </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>44934</v>
       </c>
@@ -1188,7 +535,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>44941</v>
       </c>
@@ -1211,7 +558,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>44948</v>
       </c>
@@ -1234,7 +581,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>44955</v>
       </c>
@@ -1257,7 +604,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>44962</v>
       </c>
@@ -1280,7 +627,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>44969</v>
       </c>
@@ -1303,7 +650,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>44976</v>
       </c>
@@ -1328,7 +675,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>44983</v>
       </c>
@@ -1353,7 +700,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>44990</v>
       </c>
@@ -1376,7 +723,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>44997</v>
       </c>
@@ -1399,7 +746,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>45004</v>
       </c>
@@ -1422,7 +769,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>45011</v>
       </c>
@@ -1445,7 +792,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>45018</v>
       </c>
@@ -1468,7 +815,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>45025</v>
       </c>
@@ -1491,7 +838,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>45032</v>
       </c>
@@ -1514,7 +861,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>45039</v>
       </c>
@@ -1537,7 +884,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>45046</v>
       </c>
@@ -1560,7 +907,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>45053</v>
       </c>
@@ -1583,7 +930,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>45060</v>
       </c>
@@ -1606,7 +953,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>45067</v>
       </c>
@@ -1629,7 +976,7 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>45074</v>
       </c>
@@ -1652,7 +999,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>45081</v>
       </c>
@@ -1675,7 +1022,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>45088</v>
       </c>
@@ -1698,7 +1045,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>45095</v>
       </c>
@@ -1721,7 +1068,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>45102</v>
       </c>
@@ -1744,7 +1091,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>45109</v>
       </c>
@@ -1767,7 +1114,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>45116</v>
       </c>
@@ -1790,7 +1137,7 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>45123</v>
       </c>
@@ -1813,7 +1160,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>45130</v>
       </c>
@@ -1836,7 +1183,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>45137</v>
       </c>
@@ -1859,7 +1206,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>45144</v>
       </c>
@@ -1882,7 +1229,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>45151</v>
       </c>
@@ -1905,7 +1252,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>45158</v>
       </c>
@@ -1928,7 +1275,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>45165</v>
       </c>
@@ -1951,7 +1298,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>45172</v>
       </c>
@@ -1974,7 +1321,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>45179</v>
       </c>
@@ -2001,7 +1348,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>45186</v>
       </c>
@@ -2028,7 +1375,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>45193</v>
       </c>
@@ -2055,7 +1402,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>45200</v>
       </c>
@@ -2080,7 +1427,7 @@
       </c>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>45207</v>
       </c>
@@ -2105,7 +1452,7 @@
       </c>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>45214</v>
       </c>
@@ -2130,7 +1477,7 @@
       </c>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>45221</v>
       </c>
@@ -2157,7 +1504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>45228</v>
       </c>
@@ -2180,7 +1527,7 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>45235</v>
       </c>
@@ -2203,7 +1550,7 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>45242</v>
       </c>
@@ -2226,7 +1573,7 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>45249</v>
       </c>
@@ -2249,7 +1596,7 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>45256</v>
       </c>
@@ -2272,7 +1619,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>45263</v>
       </c>
@@ -2295,7 +1642,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>45270</v>
       </c>
@@ -2318,7 +1665,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>45277</v>
       </c>
@@ -2341,7 +1688,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>45284</v>
       </c>
@@ -2364,7 +1711,7 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>45291</v>
       </c>
@@ -2387,7 +1734,7 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>45298</v>
       </c>
@@ -2408,7 +1755,7 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>45305</v>
       </c>
@@ -2429,7 +1776,7 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>45312</v>
       </c>
@@ -2450,7 +1797,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>45319</v>
       </c>
@@ -2471,7 +1818,7 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>45326</v>
       </c>
@@ -2492,7 +1839,7 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>45333</v>
       </c>
@@ -2513,7 +1860,7 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>45340</v>
       </c>
@@ -2534,7 +1881,7 @@
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>45347</v>
       </c>
@@ -2555,7 +1902,7 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>45354</v>
       </c>
@@ -2576,7 +1923,7 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>45361</v>
       </c>
@@ -2597,7 +1944,7 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>45368</v>
       </c>
@@ -2618,7 +1965,7 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>45375</v>
       </c>
@@ -2639,7 +1986,7 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>45382</v>
       </c>
@@ -2660,7 +2007,7 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>45389</v>
       </c>
@@ -2681,7 +2028,7 @@
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>45396</v>
       </c>
@@ -2702,7 +2049,7 @@
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>45403</v>
       </c>
@@ -2723,7 +2070,7 @@
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>45410</v>
       </c>
@@ -2744,7 +2091,7 @@
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>45417</v>
       </c>
@@ -2765,7 +2112,7 @@
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>45424</v>
       </c>
@@ -2786,7 +2133,7 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>45431</v>
       </c>
@@ -2807,7 +2154,7 @@
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>45438</v>
       </c>
@@ -2828,7 +2175,7 @@
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>45445</v>
       </c>
@@ -2849,7 +2196,7 @@
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>45452</v>
       </c>
@@ -2870,7 +2217,7 @@
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>45459</v>
       </c>
@@ -2891,7 +2238,7 @@
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>45466</v>
       </c>
@@ -2912,7 +2259,7 @@
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>45473</v>
       </c>
@@ -2933,7 +2280,7 @@
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>45480</v>
       </c>
@@ -2954,7 +2301,7 @@
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>45487</v>
       </c>
@@ -2975,7 +2322,7 @@
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>45494</v>
       </c>
@@ -2996,7 +2343,7 @@
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>45501</v>
       </c>
@@ -3017,7 +2364,7 @@
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>45508</v>
       </c>
@@ -3038,7 +2385,7 @@
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>45515</v>
       </c>
@@ -3059,7 +2406,7 @@
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>45522</v>
       </c>
@@ -3080,7 +2427,7 @@
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>45529</v>
       </c>
@@ -3101,7 +2448,7 @@
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
         <v>45536</v>
       </c>
@@ -3122,7 +2469,7 @@
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
         <v>45543</v>
       </c>
@@ -3143,7 +2490,7 @@
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
         <v>45550</v>
       </c>
@@ -3164,7 +2511,7 @@
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>45557</v>
       </c>
@@ -3185,7 +2532,7 @@
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>45564</v>
       </c>
@@ -3206,7 +2553,7 @@
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>45571</v>
       </c>
@@ -3227,7 +2574,7 @@
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>45578</v>
       </c>
@@ -3248,7 +2595,7 @@
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
         <v>45585</v>
       </c>
@@ -3269,7 +2616,7 @@
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>45592</v>
       </c>
@@ -3290,7 +2637,7 @@
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
         <v>45599</v>
       </c>
@@ -3311,7 +2658,7 @@
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
         <v>45606</v>
       </c>
@@ -3332,7 +2679,7 @@
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" s="3">
         <v>45613</v>
       </c>
@@ -3353,7 +2700,7 @@
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
         <v>45620</v>
       </c>
@@ -3374,7 +2721,7 @@
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
         <v>45627</v>
       </c>
@@ -3395,7 +2742,7 @@
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
         <v>45634</v>
       </c>
@@ -3416,7 +2763,7 @@
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
         <v>45641</v>
       </c>
@@ -3437,7 +2784,7 @@
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
         <v>45648</v>
       </c>
@@ -3458,7 +2805,7 @@
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
         <v>45655</v>
       </c>

</xml_diff>